<commit_message>
Add Clipped PC Analysis
</commit_message>
<xml_diff>
--- a/Tables/Table_3.xlsx
+++ b/Tables/Table_3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/collinoconnor/Desktop/Rprojects/Ap_variant_landscape/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F22A859-B17C-C245-919A-ECC447006F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA2793-64C9-D146-976B-58130F3CEA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{40709277-05FE-3345-906E-1C2B969B8CE3}"/>
+    <workbookView xWindow="39500" yWindow="780" windowWidth="38400" windowHeight="20020" xr2:uid="{40709277-05FE-3345-906E-1C2B969B8CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
-  <si>
-    <t>Genotype</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Lifestage</t>
   </si>
@@ -47,18 +44,6 @@
     <t>Adult</t>
   </si>
   <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>SCR (patch)</t>
-  </si>
-  <si>
-    <t>SCR (landscape)</t>
-  </si>
-  <si>
-    <t>v1</t>
-  </si>
-  <si>
     <t>Nymph</t>
   </si>
   <si>
@@ -66,15 +51,6 @@
   </si>
   <si>
     <t>β</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>0.006*</t>
-  </si>
-  <si>
-    <t>0.005*</t>
   </si>
   <si>
     <r>
@@ -91,6 +67,21 @@
       <t>β</t>
     </r>
   </si>
+  <si>
+    <t>Tick density</t>
+  </si>
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +91,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,11 +110,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
     </font>
     <font>
       <sz val="12"/>
@@ -191,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -205,21 +191,13 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,8 +230,8 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
@@ -623,17 +601,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E91883E-4180-8A4E-8983-33E952A6958C}">
-  <dimension ref="B4:J17"/>
+  <dimension ref="B4:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="Q29:R29"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="7.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" style="1" customWidth="1"/>
@@ -651,19 +629,19 @@
     </row>
     <row r="5" spans="3:10" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
@@ -671,7 +649,7 @@
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
@@ -682,161 +660,86 @@
     <row r="7" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.66047060000000002</v>
+      </c>
+      <c r="G7" s="7">
+        <f>EXP(F7)</f>
+        <v>1.9357030619519859</v>
+      </c>
+      <c r="H7" s="10">
+        <v>8.1469909999999993E-3</v>
+      </c>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="10">
-        <v>1.98</v>
-      </c>
-      <c r="G8" s="10">
-        <v>7.24</v>
-      </c>
-      <c r="H8" s="14">
-        <v>5.1299999999999998E-2</v>
-      </c>
-      <c r="J8" s="14">
-        <v>5.1299999999999998E-2</v>
-      </c>
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="7">
+        <v>-0.92885960000000001</v>
+      </c>
+      <c r="G8" s="7">
+        <f>EXP(F8)</f>
+        <v>0.39500391608141311</v>
+      </c>
+      <c r="H8" s="10">
+        <v>7.4490563999999995E-2</v>
+      </c>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="C9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="5"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10">
-        <v>-1.19</v>
-      </c>
-      <c r="G10" s="10">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="14">
-        <v>5.5199999999999997E-3</v>
-      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.84877499999999995</v>
+      </c>
+      <c r="G10" s="7">
+        <f>EXP(F10)</f>
+        <v>2.3367825392820643</v>
+      </c>
+      <c r="H10" s="10">
+        <v>6.9343646999999994E-2</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="5"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="10">
-        <v>0.309</v>
-      </c>
-      <c r="G11" s="10">
-        <v>1.36</v>
-      </c>
-      <c r="H11" s="14">
-        <v>0.65400000000000003</v>
-      </c>
-      <c r="J11" s="14">
-        <v>0.65400000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="H12" s="16"/>
-      <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="8"/>
-      <c r="D13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="14"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="8"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="10">
-        <v>2.04</v>
-      </c>
-      <c r="G14" s="10">
-        <v>7.69</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="14">
-        <v>5.9800000000000001E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="8"/>
-      <c r="D15" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="14"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="E16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="10">
-        <v>-1.69</v>
-      </c>
-      <c r="G16" s="10">
-        <v>0.184</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="14">
-        <v>4.6100000000000004E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="10">
-        <v>1.69</v>
-      </c>
-      <c r="G17" s="10">
-        <v>5.39</v>
-      </c>
-      <c r="H17" s="14">
-        <v>6.1499999999999999E-2</v>
-      </c>
-      <c r="J17" s="14">
-        <v>6.1499999999999999E-2</v>
+      <c r="F11" s="7">
+        <v>1.2499574</v>
+      </c>
+      <c r="G11" s="7">
+        <f>EXP(F11)</f>
+        <v>3.4901942720188761</v>
+      </c>
+      <c r="H11" s="10">
+        <v>2.3154149999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>